<commit_message>
Update of SoE tables
Updates in analysis.R meta_outcome_soe, and markdown
</commit_message>
<xml_diff>
--- a/data/included_studies_2024-01-22_LSR3_H.xlsx
+++ b/data/included_studies_2024-01-22_LSR3_H.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/LRZ Sync+Share/Projects/GALENOS/3. systematic reviews/taar/4_analysis/final_dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/Documents/GitHub/LSR3_taar1_H/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A40953-DE1C-B249-828B-B7629A231977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF4104C-928F-7C49-ABBD-678F3D76C030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19220" yWindow="-19940" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24460" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of included studies" sheetId="9" r:id="rId1"/>
@@ -826,20 +826,12 @@
     <t>Efficacy (negative symptoms), tolerability</t>
   </si>
   <si>
-    <t>Part A: Ralmitaront; placebo (monotherapy)
-Part B: Ralmitaront low or high dose; placebo (add-on to current antipsychotics)</t>
-  </si>
-  <si>
     <t>fMRI</t>
   </si>
   <si>
     <t>Pharmacokinetics</t>
   </si>
   <si>
-    <t xml:space="preserve">Cohort 1: Ulotaront 10mg; Placebo
-Cohort 2: Ulotaront 50mg; Placebo </t>
-  </si>
-  <si>
     <t>Sleep parameters, pharmacokinetics</t>
   </si>
   <si>
@@ -852,10 +844,6 @@
     <t>Efficacy (MDD), tolerability</t>
   </si>
   <si>
-    <t>Cohort 1: Ulotaront (50mg/d to 100mg/d); Placebo 
-Cohort 2: Ulotaront (25mg/d to 100mg/d); Placebo</t>
-  </si>
-  <si>
     <t>QTc interval, tolerability, pharmacokinetics</t>
   </si>
   <si>
@@ -872,6 +860,15 @@
   </si>
   <si>
     <t>Efficacy (acute), safety</t>
+  </si>
+  <si>
+    <t>Cohort 1: Ulotaront (50mg/d to 100mg/d); Placebo; Cohort 2: Ulotaront (25mg/d to 100mg/d); Placebo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cohort 1: Ulotaront 10mg; Placebo; Cohort 2: Ulotaront 50mg; Placebo </t>
+  </si>
+  <si>
+    <t>Part A: Ralmitaront; placebo (monotherapy); Part B: Ralmitaront low or high dose; placebo (add-on to current antipsychotics)</t>
   </si>
 </sst>
 </file>
@@ -1287,8 +1284,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,7 +1391,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1414,7 +1411,7 @@
         <v>76</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="H3">
         <v>128</v>
@@ -1640,7 +1637,7 @@
         <v>900</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>98</v>
@@ -1684,7 +1681,7 @@
         <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>94</v>
@@ -1766,7 +1763,7 @@
         <v>108</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="H11">
         <v>13</v>
@@ -1904,7 +1901,7 @@
         <v>52</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>94</v>
@@ -1942,13 +1939,13 @@
         <v>123</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="H15">
         <v>24</v>
       </c>
       <c r="I15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>94</v>
@@ -1992,7 +1989,7 @@
         <v>105</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J16" s="2">
         <v>41699</v>
@@ -2124,7 +2121,7 @@
         <v>18</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>132</v>
@@ -2168,7 +2165,7 @@
         <v>68</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>135</v>
@@ -2256,7 +2253,7 @@
         <v>60</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>144</v>
@@ -2300,7 +2297,7 @@
         <v>60</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>147</v>
@@ -2388,7 +2385,7 @@
         <v>36</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>155</v>
@@ -2520,7 +2517,7 @@
         <v>39</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>168</v>
@@ -2564,7 +2561,7 @@
         <v>464</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>172</v>
@@ -2740,7 +2737,7 @@
         <v>475</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>186</v>
@@ -2874,15 +2871,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9667EA7A926CE44956D0B5DCD9CC853" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d16da6adbc1ddf8797d77451e3cf87a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1d306db0-a384-4295-b85c-939a3142a74b" xmlns:ns3="a3c2bd72-a5a7-4afd-b193-b6de680f91cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b95c06a4b98ee3d310726f4e0c3474a8" ns2:_="" ns3:_="">
     <xsd:import namespace="1d306db0-a384-4295-b85c-939a3142a74b"/>
@@ -3065,21 +3053,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB39C5E6-EEF6-4ED3-A020-8D524EF8560D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E7D91A3-6CE8-4434-B49C-80EABACC49BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3098,11 +3087,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3430553F-8EDA-442D-BB5A-06A762556CDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB39C5E6-EEF6-4ED3-A020-8D524EF8560D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>